<commit_message>
Use XLSX utility functions for storage
</commit_message>
<xml_diff>
--- a/test/storage-files/data/persons.xlsx
+++ b/test/storage-files/data/persons.xlsx
@@ -20,27 +20,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t xml:space="preserve">pid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Foo Bar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">foo@bar.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Baz Quux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">baz@quux.com</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t xml:space="preserve">%pid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%Foo Bar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%foo@bar.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%Baz Quux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%baz@quux.com</t>
   </si>
 </sst>
 </file>
@@ -155,7 +161,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -179,31 +185,30 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>1</v>
+      <c r="A2" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>2</v>
+      <c r="A3" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="foo@bar.com"/>
-    <hyperlink ref="C3" r:id="rId2" display="baz@quux.com"/>
+    <hyperlink ref="C3" r:id="rId1" display="baz@quux.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>